<commit_message>
Add more calculations to power budget
</commit_message>
<xml_diff>
--- a/docs/Power Budget.xlsx
+++ b/docs/Power Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\TFT\Electrical\Singularity\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EBE045-E739-4C3B-AC11-A7DB5FD11FE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADF5F97-100D-4812-B6A0-E0D5898F2CA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
   <si>
     <t>Part</t>
   </si>
@@ -87,21 +87,12 @@
     <t>Margin</t>
   </si>
   <si>
-    <t>Power</t>
-  </si>
-  <si>
     <t>TPS62850x-Q1</t>
   </si>
   <si>
     <t>Voltage regulator</t>
   </si>
   <si>
-    <t>OBC_1V2_P</t>
-  </si>
-  <si>
-    <t>OBC_1V2_R</t>
-  </si>
-  <si>
     <t>88% efficiency</t>
   </si>
   <si>
@@ -147,23 +138,44 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Circuit area:</t>
-  </si>
-  <si>
     <t>Total power</t>
   </si>
   <si>
     <t>Rail</t>
   </si>
   <si>
-    <t>OBC_1V2</t>
+    <t>Test mode current</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t>Test mode current is used to calculate maximum current draw</t>
+  </si>
+  <si>
+    <t>as it has the highest possible current draw of all the uC modes.</t>
+  </si>
+  <si>
+    <t>Those values should not be used for thermal calculations though.</t>
+  </si>
+  <si>
+    <t>OBC_1V25</t>
+  </si>
+  <si>
+    <t>Test mode</t>
+  </si>
+  <si>
+    <t>OBC_1V25_P</t>
+  </si>
+  <si>
+    <t>OBC_1V25_R</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +203,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -200,7 +220,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -263,12 +283,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -291,35 +338,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -327,18 +347,44 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -621,7 +667,7 @@
   <dimension ref="B3:W65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,6 +675,7 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
@@ -645,76 +692,81 @@
     <col min="21" max="21" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="O4" s="20" t="s">
+    <row r="3" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="6"/>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="22">
+      <c r="C4" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="13">
         <v>0.88</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="T4" s="14">
+      <c r="T4" s="26">
         <v>0.2</v>
       </c>
-      <c r="U4" s="15"/>
+      <c r="U4" s="27"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="19"/>
+      <c r="F5" s="32"/>
       <c r="L5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="M5" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
       <c r="Q5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R5" s="13" t="s">
+      <c r="R5" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
     </row>
     <row r="6" spans="2:23" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="12"/>
+      <c r="D6" s="24"/>
       <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="G6" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="H6" s="9"/>
       <c r="I6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="12"/>
+      <c r="K6" s="24"/>
       <c r="L6" s="2" t="s">
         <v>2</v>
       </c>
@@ -747,14 +799,14 @@
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>25</v>
+      <c r="B7" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>22</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E7" s="5">
         <v>195</v>
@@ -762,15 +814,18 @@
       <c r="F7" s="5">
         <v>380</v>
       </c>
-      <c r="H7" s="29"/>
-      <c r="I7" s="16" t="s">
+      <c r="G7">
+        <v>475</v>
+      </c>
+      <c r="H7" s="19"/>
+      <c r="I7" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="16" t="s">
-        <v>19</v>
-      </c>
       <c r="K7" s="5" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="L7" s="5">
         <v>3.3</v>
@@ -786,37 +841,37 @@
         <v>260</v>
       </c>
       <c r="P7" s="5">
-        <f>SUM(F7:F12)</f>
-        <v>445</v>
+        <f>SUM(G7:G12)</f>
+        <v>540</v>
       </c>
       <c r="Q7" s="5">
         <v>1.25</v>
       </c>
-      <c r="R7" s="23">
+      <c r="R7" s="14">
         <f>(O7/1000*$Q7*(1/$Q$4-1)+M7/1000*$L7)*1000</f>
         <v>44.374281818181856</v>
       </c>
-      <c r="S7" s="23">
+      <c r="S7" s="14">
         <f>(P7/1000*$Q7*(1/$Q$4-1)+N7/1000*$L7)*1000</f>
-        <v>75.971072727272784</v>
-      </c>
-      <c r="T7" s="23">
+        <v>92.164254545454625</v>
+      </c>
+      <c r="T7" s="14">
         <f>R7*(1+$T$4)</f>
         <v>53.249138181818225</v>
       </c>
-      <c r="U7" s="23">
+      <c r="U7" s="14">
         <f>S7*(1+$T$4)</f>
-        <v>91.16528727272734</v>
+        <v>110.59710545454554</v>
       </c>
       <c r="W7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E8" s="6">
         <v>10</v>
@@ -824,11 +879,14 @@
       <c r="F8" s="6">
         <v>10</v>
       </c>
-      <c r="H8" s="29"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8" s="19"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
       <c r="K8" s="6" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="L8" s="6">
         <v>3.3</v>
@@ -848,28 +906,28 @@
       <c r="Q8" s="6">
         <v>1.25</v>
       </c>
-      <c r="R8" s="24">
+      <c r="R8" s="15">
         <f>(O8/1000*$Q8*(1/$Q$4-1)+M8/1000*$L8)*1000</f>
         <v>5.6099999999999997E-2</v>
       </c>
-      <c r="S8" s="24">
+      <c r="S8" s="15">
         <f>(P8/1000*$Q8*(1/$Q$4-1)+N8/1000*$L8)*1000</f>
         <v>0.11879999999999998</v>
       </c>
-      <c r="T8" s="24">
-        <f t="shared" ref="T7:T8" si="0">R8*(1+$T$4)</f>
+      <c r="T8" s="15">
+        <f t="shared" ref="T8" si="0">R8*(1+$T$4)</f>
         <v>6.7319999999999991E-2</v>
       </c>
-      <c r="U8" s="24">
-        <f t="shared" ref="U7:U8" si="1">S8*(1+$T$4)</f>
+      <c r="U8" s="15">
+        <f t="shared" ref="U8" si="1">S8*(1+$T$4)</f>
         <v>0.14255999999999996</v>
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E9" s="6">
         <v>0</v>
@@ -877,12 +935,15 @@
       <c r="F9" s="6">
         <v>0</v>
       </c>
-      <c r="H9" s="29"/>
-      <c r="I9" s="25" t="s">
-        <v>34</v>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="19"/>
+      <c r="I9" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6">
@@ -895,37 +956,37 @@
         <v>0</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q9" s="24">
+        <v>42</v>
+      </c>
+      <c r="Q9" s="15">
         <f>Q7-(P7*0.14/1000)</f>
-        <v>1.1877</v>
-      </c>
-      <c r="R9" s="24">
+        <v>1.1743999999999999</v>
+      </c>
+      <c r="R9" s="15">
         <f>POWER(O7/1000,2)*0.14*1000</f>
         <v>9.4640000000000022</v>
       </c>
-      <c r="S9" s="24">
+      <c r="S9" s="15">
         <f>POWER(P7/1000,2)*0.14*1000</f>
-        <v>27.723500000000005</v>
-      </c>
-      <c r="T9" s="24">
+        <v>40.824000000000005</v>
+      </c>
+      <c r="T9" s="15">
         <f>R9*(1+$T$4)</f>
         <v>11.356800000000002</v>
       </c>
-      <c r="U9" s="24">
+      <c r="U9" s="15">
         <f>S9*(1+$T$4)</f>
-        <v>33.268200000000007</v>
+        <v>48.988800000000005</v>
       </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E10" s="6">
         <v>0</v>
@@ -933,26 +994,34 @@
       <c r="F10" s="6">
         <v>0</v>
       </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="19"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q10" s="15">
+        <f>Q7-(SUM(F7:F12)*0.14/1000)</f>
+        <v>1.1877</v>
+      </c>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E11" s="6">
         <v>0</v>
@@ -960,26 +1029,34 @@
       <c r="F11" s="6">
         <v>0</v>
       </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
       <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="33">
+        <f>Q7-(O7*0.14/1000)</f>
+        <v>1.2136</v>
+      </c>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E12" s="7">
         <v>55</v>
@@ -987,80 +1064,97 @@
       <c r="F12" s="7">
         <v>55</v>
       </c>
-      <c r="Q12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="R12" s="26">
+      <c r="G12" s="7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="I13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R13" s="17">
         <f>SUM(R7:R9)</f>
         <v>53.894381818181856</v>
       </c>
-      <c r="S12" s="26">
-        <f t="shared" ref="S12:U12" si="2">SUM(S7:S9)</f>
-        <v>103.81337272727278</v>
-      </c>
-      <c r="T12" s="26">
-        <f t="shared" si="2"/>
+      <c r="S13" s="17">
+        <f>SUM(S7:S9)</f>
+        <v>133.10705454545462</v>
+      </c>
+      <c r="T13" s="17">
+        <f>SUM(T7:T9)</f>
         <v>64.673258181818227</v>
       </c>
-      <c r="U12" s="27">
-        <f t="shared" si="2"/>
-        <v>124.57604727272735</v>
-      </c>
-    </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
+      <c r="U13" s="18">
+        <f>SUM(U7:U9)</f>
+        <v>159.72846545454556</v>
+      </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="17">
+        <f>SUM(E7:E12)*$Q$9</f>
+        <v>305.34399999999999</v>
+      </c>
+      <c r="F14" s="17">
+        <f>SUM(F7:F12)*$Q$9</f>
+        <v>522.60799999999995</v>
+      </c>
+      <c r="G14" s="18">
+        <f>SUM(G7:G12)*$Q$9</f>
+        <v>634.17599999999993</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="31" t="s">
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="J15" s="20" t="s">
         <v>40</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="26">
-        <f>SUM(E7:E12)*$Q$9</f>
-        <v>308.80200000000002</v>
-      </c>
-      <c r="F14" s="27">
-        <f>SUM(F7:F12)*$Q$9</f>
-        <v>528.52649999999994</v>
-      </c>
-      <c r="G14" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="57" spans="8:21" x14ac:dyDescent="0.25">
       <c r="S57" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="T57" s="14">
+      <c r="T57" s="26">
         <v>0.2</v>
       </c>
-      <c r="U57" s="15"/>
+      <c r="U57" s="27"/>
     </row>
     <row r="58" spans="8:21" x14ac:dyDescent="0.25">
       <c r="L58" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M58" s="13" t="s">
+      <c r="M58" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="N58" s="13"/>
-      <c r="O58" s="13"/>
-      <c r="P58" s="13"/>
+      <c r="N58" s="25"/>
+      <c r="O58" s="25"/>
+      <c r="P58" s="25"/>
       <c r="Q58" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R58" s="13" t="s">
+      <c r="R58" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="S58" s="13"/>
-      <c r="T58" s="13"/>
-      <c r="U58" s="13"/>
+      <c r="S58" s="25"/>
+      <c r="T58" s="25"/>
+      <c r="U58" s="25"/>
     </row>
     <row r="59" spans="8:21" ht="30" x14ac:dyDescent="0.25">
       <c r="H59" s="2" t="s">
@@ -1069,10 +1163,10 @@
       <c r="I59" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J59" s="12" t="s">
+      <c r="J59" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="K59" s="12"/>
+      <c r="K59" s="24"/>
       <c r="L59" s="2" t="s">
         <v>2</v>
       </c>
@@ -1105,17 +1199,17 @@
       </c>
     </row>
     <row r="60" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H60" s="16" t="s">
+      <c r="H60" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="I60" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J60" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="K60" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="I60" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="J60" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="K60" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="L60" s="5">
         <v>1.2</v>
@@ -1130,20 +1224,20 @@
       <c r="R60" s="5"/>
       <c r="S60" s="5"/>
       <c r="T60" s="5">
-        <f>R60*$T$57</f>
+        <f t="shared" ref="T60:U65" si="2">R60*$T$57</f>
         <v>0</v>
       </c>
       <c r="U60" s="5">
-        <f>S60*$T$57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
-      <c r="J61" s="17"/>
+      <c r="H61" s="29"/>
+      <c r="I61" s="29"/>
+      <c r="J61" s="29"/>
       <c r="K61" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L61" s="6">
         <v>1.2</v>
@@ -1156,20 +1250,20 @@
       <c r="R61" s="6"/>
       <c r="S61" s="6"/>
       <c r="T61" s="6">
-        <f>R61*$T$57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U61" s="6">
-        <f>S61*$T$57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H62" s="17"/>
-      <c r="I62" s="17"/>
-      <c r="J62" s="17"/>
+      <c r="H62" s="29"/>
+      <c r="I62" s="29"/>
+      <c r="J62" s="29"/>
       <c r="K62" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L62" s="6">
         <v>1.2</v>
@@ -1182,20 +1276,20 @@
       <c r="R62" s="6"/>
       <c r="S62" s="6"/>
       <c r="T62" s="6">
-        <f>R62*$T$57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U62" s="6">
-        <f>S62*$T$57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H63" s="17"/>
-      <c r="I63" s="17"/>
-      <c r="J63" s="17"/>
+      <c r="H63" s="29"/>
+      <c r="I63" s="29"/>
+      <c r="J63" s="29"/>
       <c r="K63" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L63" s="8">
         <v>1.2</v>
@@ -1208,20 +1302,20 @@
       <c r="R63" s="6"/>
       <c r="S63" s="6"/>
       <c r="T63" s="6">
-        <f>R63*$T$57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U63" s="6">
-        <f>S63*$T$57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H64" s="17"/>
-      <c r="I64" s="17"/>
-      <c r="J64" s="17"/>
+      <c r="H64" s="29"/>
+      <c r="I64" s="29"/>
+      <c r="J64" s="29"/>
       <c r="K64" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L64" s="8">
         <v>1.2</v>
@@ -1234,20 +1328,20 @@
       <c r="R64" s="6"/>
       <c r="S64" s="6"/>
       <c r="T64" s="6">
-        <f>R64*$T$57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U64" s="6">
-        <f>S64*$T$57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H65" s="12"/>
-      <c r="I65" s="12"/>
-      <c r="J65" s="12"/>
+      <c r="H65" s="24"/>
+      <c r="I65" s="24"/>
+      <c r="J65" s="24"/>
       <c r="K65" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L65" s="11">
         <v>1.2</v>
@@ -1260,11 +1354,11 @@
       <c r="R65" s="7"/>
       <c r="S65" s="7"/>
       <c r="T65" s="7">
-        <f>R65*$T$57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U65" s="7">
-        <f>S65*$T$57</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix power budget math
</commit_message>
<xml_diff>
--- a/docs/Power Budget.xlsx
+++ b/docs/Power Budget.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\TFT\Electrical\Singularity\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADF5F97-100D-4812-B6A0-E0D5898F2CA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C72AB3-9602-4C5C-8CE7-8579E1B063A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -354,34 +354,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -667,7 +667,7 @@
   <dimension ref="B3:W65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,53 +703,53 @@
       <c r="C4" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="O4" s="30" t="s">
+      <c r="O4" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="P4" s="31"/>
+      <c r="P4" s="33"/>
       <c r="Q4" s="13">
         <v>0.88</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="T4" s="26">
+      <c r="T4" s="29">
         <v>0.2</v>
       </c>
-      <c r="U4" s="27"/>
+      <c r="U4" s="30"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="28"/>
       <c r="L5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="25" t="s">
+      <c r="M5" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
       <c r="Q5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R5" s="25" t="s">
+      <c r="R5" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
     </row>
     <row r="6" spans="2:23" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="24"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
@@ -763,10 +763,10 @@
       <c r="I6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="24" t="s">
+      <c r="J6" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="24"/>
+      <c r="K6" s="25"/>
       <c r="L6" s="2" t="s">
         <v>2</v>
       </c>
@@ -799,10 +799,10 @@
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="26" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -818,10 +818,10 @@
         <v>475</v>
       </c>
       <c r="H7" s="19"/>
-      <c r="I7" s="28" t="s">
+      <c r="I7" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="28" t="s">
+      <c r="J7" s="26" t="s">
         <v>18</v>
       </c>
       <c r="K7" s="5" t="s">
@@ -848,28 +848,28 @@
         <v>1.25</v>
       </c>
       <c r="R7" s="14">
-        <f>(O7/1000*$Q7*(1/$Q$4-1)+M7/1000*$L7)*1000</f>
-        <v>44.374281818181856</v>
+        <f>(O7/1000*$Q7*(1-$Q$4)+M7/1000*$L7)*1000</f>
+        <v>39.056100000000001</v>
       </c>
       <c r="S7" s="14">
-        <f>(P7/1000*$Q7*(1/$Q$4-1)+N7/1000*$L7)*1000</f>
-        <v>92.164254545454625</v>
+        <f>(P7/1000*$Q7*(1-$Q$4)+N7/1000*$L7)*1000</f>
+        <v>81.118800000000007</v>
       </c>
       <c r="T7" s="14">
         <f>R7*(1+$T$4)</f>
-        <v>53.249138181818225</v>
+        <v>46.867319999999999</v>
       </c>
       <c r="U7" s="14">
         <f>S7*(1+$T$4)</f>
-        <v>110.59710545454554</v>
+        <v>97.342560000000006</v>
       </c>
       <c r="W7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="6" t="s">
         <v>28</v>
       </c>
@@ -883,8 +883,8 @@
         <v>10</v>
       </c>
       <c r="H8" s="19"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
       <c r="K8" s="6" t="s">
         <v>44</v>
       </c>
@@ -907,11 +907,11 @@
         <v>1.25</v>
       </c>
       <c r="R8" s="15">
-        <f>(O8/1000*$Q8*(1/$Q$4-1)+M8/1000*$L8)*1000</f>
+        <f>(O8/1000*$Q8*(1-$Q$4)+M8/1000*$L8)*1000</f>
         <v>5.6099999999999997E-2</v>
       </c>
       <c r="S8" s="15">
-        <f>(P8/1000*$Q8*(1/$Q$4-1)+N8/1000*$L8)*1000</f>
+        <f>(P8/1000*$Q8*(1-$Q$4)+N8/1000*$L8)*1000</f>
         <v>0.11879999999999998</v>
       </c>
       <c r="T8" s="15">
@@ -924,8 +924,8 @@
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="6" t="s">
         <v>24</v>
       </c>
@@ -983,8 +983,8 @@
       </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="6" t="s">
         <v>25</v>
       </c>
@@ -1018,8 +1018,8 @@
       <c r="U10" s="6"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="6" t="s">
         <v>26</v>
       </c>
@@ -1043,7 +1043,7 @@
       <c r="P11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="Q11" s="33">
+      <c r="Q11" s="24">
         <f>Q7-(O7*0.14/1000)</f>
         <v>1.2136</v>
       </c>
@@ -1053,8 +1053,8 @@
       <c r="U11" s="7"/>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="7" t="s">
         <v>27</v>
       </c>
@@ -1082,19 +1082,19 @@
       </c>
       <c r="R13" s="17">
         <f>SUM(R7:R9)</f>
-        <v>53.894381818181856</v>
+        <v>48.5762</v>
       </c>
       <c r="S13" s="17">
         <f>SUM(S7:S9)</f>
-        <v>133.10705454545462</v>
+        <v>122.0616</v>
       </c>
       <c r="T13" s="17">
         <f>SUM(T7:T9)</f>
-        <v>64.673258181818227</v>
+        <v>58.291440000000001</v>
       </c>
       <c r="U13" s="18">
         <f>SUM(U7:U9)</f>
-        <v>159.72846545454556</v>
+        <v>146.47392000000002</v>
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.25">
@@ -1131,30 +1131,30 @@
       <c r="S57" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="T57" s="26">
+      <c r="T57" s="29">
         <v>0.2</v>
       </c>
-      <c r="U57" s="27"/>
+      <c r="U57" s="30"/>
     </row>
     <row r="58" spans="8:21" x14ac:dyDescent="0.25">
       <c r="L58" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M58" s="25" t="s">
+      <c r="M58" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="N58" s="25"/>
-      <c r="O58" s="25"/>
-      <c r="P58" s="25"/>
+      <c r="N58" s="31"/>
+      <c r="O58" s="31"/>
+      <c r="P58" s="31"/>
       <c r="Q58" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R58" s="25" t="s">
+      <c r="R58" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="S58" s="25"/>
-      <c r="T58" s="25"/>
-      <c r="U58" s="25"/>
+      <c r="S58" s="31"/>
+      <c r="T58" s="31"/>
+      <c r="U58" s="31"/>
     </row>
     <row r="59" spans="8:21" ht="30" x14ac:dyDescent="0.25">
       <c r="H59" s="2" t="s">
@@ -1163,10 +1163,10 @@
       <c r="I59" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J59" s="24" t="s">
+      <c r="J59" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="K59" s="24"/>
+      <c r="K59" s="25"/>
       <c r="L59" s="2" t="s">
         <v>2</v>
       </c>
@@ -1199,13 +1199,13 @@
       </c>
     </row>
     <row r="60" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H60" s="28" t="s">
+      <c r="H60" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="I60" s="28" t="s">
+      <c r="I60" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="J60" s="28" t="s">
+      <c r="J60" s="26" t="s">
         <v>22</v>
       </c>
       <c r="K60" s="5" t="s">
@@ -1233,9 +1233,9 @@
       </c>
     </row>
     <row r="61" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H61" s="29"/>
-      <c r="I61" s="29"/>
-      <c r="J61" s="29"/>
+      <c r="H61" s="27"/>
+      <c r="I61" s="27"/>
+      <c r="J61" s="27"/>
       <c r="K61" s="6" t="s">
         <v>28</v>
       </c>
@@ -1259,9 +1259,9 @@
       </c>
     </row>
     <row r="62" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H62" s="29"/>
-      <c r="I62" s="29"/>
-      <c r="J62" s="29"/>
+      <c r="H62" s="27"/>
+      <c r="I62" s="27"/>
+      <c r="J62" s="27"/>
       <c r="K62" s="6" t="s">
         <v>24</v>
       </c>
@@ -1285,9 +1285,9 @@
       </c>
     </row>
     <row r="63" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H63" s="29"/>
-      <c r="I63" s="29"/>
-      <c r="J63" s="29"/>
+      <c r="H63" s="27"/>
+      <c r="I63" s="27"/>
+      <c r="J63" s="27"/>
       <c r="K63" s="8" t="s">
         <v>25</v>
       </c>
@@ -1311,9 +1311,9 @@
       </c>
     </row>
     <row r="64" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H64" s="29"/>
-      <c r="I64" s="29"/>
-      <c r="J64" s="29"/>
+      <c r="H64" s="27"/>
+      <c r="I64" s="27"/>
+      <c r="J64" s="27"/>
       <c r="K64" s="8" t="s">
         <v>26</v>
       </c>
@@ -1337,9 +1337,9 @@
       </c>
     </row>
     <row r="65" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="H65" s="24"/>
-      <c r="I65" s="24"/>
-      <c r="J65" s="24"/>
+      <c r="H65" s="25"/>
+      <c r="I65" s="25"/>
+      <c r="J65" s="25"/>
       <c r="K65" s="11" t="s">
         <v>27</v>
       </c>
@@ -1364,17 +1364,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:C12"/>
-    <mergeCell ref="B7:B12"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="I60:I65"/>
-    <mergeCell ref="H60:H65"/>
-    <mergeCell ref="J60:J65"/>
-    <mergeCell ref="T57:U57"/>
-    <mergeCell ref="M58:P58"/>
-    <mergeCell ref="R58:U58"/>
-    <mergeCell ref="J59:K59"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="M5:P5"/>
     <mergeCell ref="R5:U5"/>
@@ -1382,6 +1371,17 @@
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="O4:P4"/>
+    <mergeCell ref="J60:J65"/>
+    <mergeCell ref="T57:U57"/>
+    <mergeCell ref="M58:P58"/>
+    <mergeCell ref="R58:U58"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="I60:I65"/>
+    <mergeCell ref="H60:H65"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>